<commit_message>
added test with excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calvario31/Documents/Projects/Appium/AppiumFramework/src/test/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calvario31/Documents/Projects/Appium/AppiumClase/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C7257F-9F56-3349-8A1F-21AE00A93F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EADE0C4-CC5A-CE44-A218-D9141937DB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="itemData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="errorMessages" sheetId="4" r:id="rId3"/>
+    <sheet name="errorInfoMessages" sheetId="4" r:id="rId2"/>
+    <sheet name="credentialsErrorMessages" sheetId="5" r:id="rId3"/>
     <sheet name="credentials" sheetId="2" r:id="rId4"/>
     <sheet name="urls" sheetId="3" r:id="rId5"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>key</t>
   </si>
@@ -170,6 +170,24 @@
   </si>
   <si>
     <t>Error: Postal Code is required</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>hola_mundo</t>
+  </si>
+  <si>
+    <t>adios_mundo</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Username and password do not match any user in this service.</t>
+  </si>
+  <si>
+    <t>Sorry, this user has been locked out.</t>
   </si>
 </sst>
 </file>
@@ -233,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -271,11 +289,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -295,6 +326,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView zoomScale="343" zoomScaleNormal="343" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="343" zoomScaleNormal="343" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1612,23 +1650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126D55C0-2E4D-724A-993C-98827ACFFCAB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="300" zoomScaleNormal="300" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2923B0-F226-6E4E-B6A0-DB50F803B91C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1674,11 +1700,55 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5F41142-F6C4-8E49-96E9-8771AA01C52C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="46.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1691,55 +1761,66 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="12" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2735,8 +2816,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:B5"/>
+    <sheetView showGridLines="0" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>